<commit_message>
updating changes related to jenkins run
</commit_message>
<xml_diff>
--- a/nopcommerceJavaSeleniumProj/src/main/java/testData/TestData.xlsx
+++ b/nopcommerceJavaSeleniumProj/src/main/java/testData/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="14">
   <si>
     <t>admin@yourstore.com</t>
   </si>
@@ -96,7 +96,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="418">
+  <borders count="450">
     <border>
       <left/>
       <right/>
@@ -1991,11 +1991,155 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2103,6 +2247,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="409" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="413" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="417" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="421" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="425" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="429" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="433" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="437" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="441" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="445" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="449" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2420,7 +2572,7 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="103">
+      <c r="D2" t="s" s="111">
         <v>5</v>
       </c>
     </row>
@@ -2434,7 +2586,7 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="104">
+      <c r="D3" t="s" s="112">
         <v>5</v>
       </c>
     </row>
@@ -2448,7 +2600,7 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="105">
+      <c r="D4" t="s" s="113">
         <v>5</v>
       </c>
     </row>
@@ -2462,7 +2614,7 @@
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s" s="106">
+      <c r="D5" t="s" s="114">
         <v>5</v>
       </c>
     </row>

</xml_diff>